<commit_message>
update tien dam cuoi
</commit_message>
<xml_diff>
--- a/Tiendamcuoi.xlsx
+++ b/Tiendamcuoi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitProjects\PersonalData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PersonalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4A447A-539E-49B7-800E-34A1DCF3ECEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8063601-863C-4377-919D-3A1242726D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anh em họ hàng" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Anh Hải Phấn</t>
   </si>
@@ -170,6 +170,27 @@
   </si>
   <si>
     <t>Anh Trọng</t>
+  </si>
+  <si>
+    <t>Đức(FPT)</t>
+  </si>
+  <si>
+    <t>Tuấn Anh (MOnkey)</t>
+  </si>
+  <si>
+    <t>Thủy(Monkey)</t>
+  </si>
+  <si>
+    <t>Trường Nhung</t>
+  </si>
+  <si>
+    <t>Lịch Tời</t>
+  </si>
+  <si>
+    <t>Anh Cường(Bác Bộc)</t>
+  </si>
+  <si>
+    <t>Anh Cao()</t>
   </si>
 </sst>
 </file>
@@ -488,15 +509,15 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +525,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -512,7 +533,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -520,13 +541,29 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="B24">
         <f>SUM(B1:B23)</f>
-        <v>1200000</v>
+        <v>2700000</v>
       </c>
     </row>
   </sheetData>
@@ -538,17 +575,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -556,7 +593,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -564,7 +601,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -572,7 +609,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -580,7 +617,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -588,7 +625,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -596,17 +633,17 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -614,7 +651,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -622,7 +659,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -630,7 +667,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -638,12 +675,12 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -651,7 +688,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -659,7 +696,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -667,7 +704,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -675,7 +712,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -683,7 +720,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -691,7 +728,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -699,7 +736,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -707,7 +744,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -715,7 +752,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -723,7 +760,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -746,17 +783,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -764,7 +801,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -772,7 +809,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -780,7 +817,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -788,13 +825,29 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
       <c r="B15">
         <f>SUM(B1:B14)</f>
-        <v>2000000</v>
+        <v>3000000</v>
       </c>
     </row>
   </sheetData>
@@ -807,15 +860,16 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -823,7 +877,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -831,7 +885,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -839,7 +893,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -847,18 +901,36 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
       <c r="B16">
         <f>SUM(B1:B10)</f>
-        <v>1800000</v>
+        <v>2300000</v>
       </c>
     </row>
   </sheetData>
@@ -868,19 +940,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -888,7 +960,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -896,7 +968,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -904,7 +976,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -912,31 +984,37 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B13">
-        <f>SUM(B1:B12)</f>
-        <v>2300000</v>
+      <c r="B17">
+        <f>SUM(B1:B16)</f>
+        <v>2900000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>